<commit_message>
Updated model estimation procedure (v0.13)
</commit_message>
<xml_diff>
--- a/model-inputs/forecasts.xlsx
+++ b/model-inputs/forecasts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive\__Projects\econforecasting\model-inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BBDE10-B77A-495D-B3B8-5901637F7207}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3856CB-1AE3-49C2-BCD0-7047CCE9AA2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5917CAB-2590-4FE1-9E2D-85810580C73C}"/>
   </bookViews>
   <sheets>
     <sheet name="params" sheetId="4" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2173" uniqueCount="383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2173" uniqueCount="382">
   <si>
     <t>gdp</t>
   </si>
@@ -1147,9 +1147,6 @@
   </si>
   <si>
     <t>CIVPART</t>
-  </si>
-  <si>
-    <t>log</t>
   </si>
   <si>
     <t>sales</t>
@@ -1253,92 +1250,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="44">
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="38">
     <dxf>
       <font>
         <b val="0"/>
@@ -1582,6 +1494,25 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1846,6 +1777,32 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <color theme="9"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1860,45 +1817,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N100" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0331C90B-C1E4-469A-92B6-B6D7D2A881B0}" name="Table13" displayName="Table13" ref="A1:N100" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
   <autoFilter ref="A1:N100" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="41"/>
-    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="40"/>
-    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="39"/>
-    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="36"/>
-    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="34"/>
-    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="32"/>
-    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="31"/>
-    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="30"/>
-    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="28"/>
+    <tableColumn id="1" xr3:uid="{67EE8FF2-8326-4684-84E6-A964C24850DB}" name="varname" dataDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{BE8BE91C-06D5-4A47-9123-C26507EAC1EF}" name="fullname" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{68FBD5CC-20E0-4926-A7D1-2E69FB0B202F}" name="category" dataDxfId="29"/>
+    <tableColumn id="14" xr3:uid="{C9DF87B4-A1B3-4AF8-A08F-43A957A887B8}" name="dispgroup" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{10A8B47F-5D16-4D4A-AADC-3A1373D3388E}" name="source" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{9D6367F7-B418-4D74-8BBC-8A868648619D}" name="sckey" dataDxfId="26"/>
+    <tableColumn id="12" xr3:uid="{B018E0B7-9E0D-4372-82AB-44595FD99EA4}" name="units" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{6FA3E542-D9A3-44CC-8D78-768A77B7C6D6}" name="freq" dataDxfId="24"/>
+    <tableColumn id="10" xr3:uid="{39B1664D-8A0F-423F-962A-A1C7C847E7B1}" name="sa" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{F5127FE9-910F-4EAC-83AB-E5C9C27639E9}" name="st" dataDxfId="22"/>
+    <tableColumn id="13" xr3:uid="{CB532FB1-25A0-4F3F-8676-01484C877F99}" name="d1" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{5C5C4553-B818-4BED-AC86-DABB94FCA34E}" name="d2" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{31F7F51C-B4E4-41E3-A390-C9AA6D66ACA0}" name="dfminput" dataDxfId="19"/>
+    <tableColumn id="5" xr3:uid="{7BA92187-1BDA-4F9D-BCE7-5391BF21BC5B}" name="nowcast" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:M88" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B0809632-345D-4118-A064-2695E36114FC}" name="Table132" displayName="Table132" ref="A1:M88" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:M88" xr:uid="{EC6D9A60-7AF3-4545-B540-E43EAD70DF9B}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="25"/>
-    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="21"/>
-    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="19"/>
-    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="18"/>
-    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="stat" dataDxfId="17"/>
-    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="disp" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="disp2" dataDxfId="15"/>
-    <tableColumn id="8" xr3:uid="{790E276A-478E-4C37-8E23-268EBECBD586}" name="dfminput" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{D4ABD328-708F-41CD-A15C-D1F52F9E510D}" name="nowcast" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{7C3A592C-91B3-4EB1-890C-6A27C315E04F}" name="varname" dataDxfId="12"/>
+    <tableColumn id="9" xr3:uid="{9C9AE510-55AD-4974-AE7E-941FC82A80BD}" name="fullname" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{D359572A-B92E-4EFE-A4E9-D570E99C652A}" name="category" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{62F8B61F-9557-4FD9-BB7B-F9CA010F3C63}" name="source" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{67A7B928-8F8D-4E54-9FCC-AF03890D139D}" name="sckey" dataDxfId="8"/>
+    <tableColumn id="12" xr3:uid="{C8C9F652-7467-441F-A98D-BE40F0F1C4FF}" name="units" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{0CA7CCC5-E59A-4121-9AFE-711B10583A49}" name="freq" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{177B6D70-8BA8-4397-98F9-95E9F55460C8}" name="sa" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{AB8672B6-1869-4430-98D0-EC6FCA5E930A}" name="stat" dataDxfId="4"/>
+    <tableColumn id="13" xr3:uid="{9F74B296-6910-4B5A-AB43-F8422ADF4F24}" name="disp" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{20D61120-4001-4E6F-92C9-AA6FB68AE34D}" name="disp2" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{790E276A-478E-4C37-8E23-268EBECBD586}" name="dfminput" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{D4ABD328-708F-41CD-A15C-D1F52F9E510D}" name="nowcast" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2203,8 +2160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BE13241-3AD3-4AF9-83CF-1259D998F1D6}">
   <dimension ref="A1:N100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M75" sqref="M75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4603,7 +4560,7 @@
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B55" s="5" t="s">
         <v>353</v>
@@ -4647,10 +4604,10 @@
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="B56" s="5" t="s">
         <v>380</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>381</v>
       </c>
       <c r="C56" s="6" t="s">
         <v>337</v>
@@ -4662,7 +4619,7 @@
         <v>178</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="G56" s="7" t="s">
         <v>339</v>
@@ -4683,7 +4640,7 @@
         <v>311</v>
       </c>
       <c r="M56" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N56" s="6" t="s">
         <v>170</v>
@@ -5378,7 +5335,7 @@
         <v>0</v>
       </c>
       <c r="J72" s="6" t="s">
-        <v>370</v>
+        <v>29</v>
       </c>
       <c r="K72" s="6" t="s">
         <v>30</v>
@@ -5510,7 +5467,7 @@
         <v>0</v>
       </c>
       <c r="J75" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K75" s="6" t="s">
         <v>30</v>
@@ -5926,7 +5883,7 @@
         <v>68</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C85" s="6" t="s">
         <v>184</v>
@@ -5959,7 +5916,7 @@
         <v>311</v>
       </c>
       <c r="M85" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N85" s="6" t="s">
         <v>170</v>
@@ -5967,7 +5924,7 @@
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B86" s="5" t="s">
         <v>108</v>
@@ -5982,7 +5939,7 @@
         <v>178</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="G86" s="7" t="s">
         <v>111</v>
@@ -6102,7 +6059,7 @@
         <v>254</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C89" s="6" t="s">
         <v>181</v>
@@ -6583,10 +6540,10 @@
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C100" s="6" t="s">
         <v>337</v>
@@ -6598,10 +6555,10 @@
         <v>178</v>
       </c>
       <c r="F100" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="G100" s="7" t="s">
         <v>377</v>
-      </c>
-      <c r="G100" s="7" t="s">
-        <v>378</v>
       </c>
       <c r="H100" s="6" t="s">
         <v>44</v>
@@ -6627,20 +6584,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="N2:N100">
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="37" priority="4">
       <formula>$M2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M100">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="35" priority="3">
       <formula>$H2 = "q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="2" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9817,17 +9774,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="M2:M88">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="17" priority="3">
       <formula>$L2=TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L88">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="16" priority="2">
       <formula>$G2 = "q"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M1:M1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="equal">
       <formula>"calc"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>